<commit_message>
Laatste post wordt nu getoond in activediscussions.
</commit_message>
<xml_diff>
--- a/Documentatie/TODO - adhv feedback hans.xlsx
+++ b/Documentatie/TODO - adhv feedback hans.xlsx
@@ -201,12 +201,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -243,6 +249,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -546,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +569,7 @@
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -567,7 +577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -575,7 +585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -583,7 +593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -591,7 +601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -599,7 +609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -607,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -615,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
@@ -623,7 +633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
@@ -631,7 +641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -639,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
@@ -647,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
@@ -655,15 +665,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
@@ -671,7 +682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Brandbox is nu beheerbaar, WHOEHOEHOE.
</commit_message>
<xml_diff>
--- a/Documentatie/TODO - adhv feedback hans.xlsx
+++ b/Documentatie/TODO - adhv feedback hans.xlsx
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -254,6 +254,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,7 +562,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,10 +629,11 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inschrijflink is foetsie, inlogtekst is beheerbaar!
</commit_message>
<xml_diff>
--- a/Documentatie/TODO - adhv feedback hans.xlsx
+++ b/Documentatie/TODO - adhv feedback hans.xlsx
@@ -562,7 +562,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,10 +662,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Er staat nu 'Quote van: ' bij een quote, nou joepie.
</commit_message>
<xml_diff>
--- a/Documentatie/TODO - adhv feedback hans.xlsx
+++ b/Documentatie/TODO - adhv feedback hans.xlsx
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -256,6 +256,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -562,7 +565,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +683,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Membername wordt nu bij notities getoond!!!
</commit_message>
<xml_diff>
--- a/Documentatie/TODO - adhv feedback hans.xlsx
+++ b/Documentatie/TODO - adhv feedback hans.xlsx
@@ -254,9 +254,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -276,6 +273,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +581,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,10 +599,10 @@
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="14"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="14"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -611,7 +611,7 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -620,7 +620,7 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -629,7 +629,7 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -638,7 +638,7 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -647,7 +647,7 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -656,17 +656,17 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -675,7 +675,7 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -684,7 +684,7 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -693,85 +693,86 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="14"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="14"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="14"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="14"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="14"/>
+      <c r="D23" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>